<commit_message>
corregido min p center
</commit_message>
<xml_diff>
--- a/Docs importantes/objectives.xlsx
+++ b/Docs importantes/objectives.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Investigacion-maxima-diversidad\Docs importantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393C067A-49D4-467E-9BD4-9F15A0154EF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D70044-4771-4E24-AC10-2CB411FADB19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F8ECD58-FE5C-4942-AC5F-309EB15FE9EC}"/>
   </bookViews>
@@ -167,7 +167,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>136</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -209,7 +209,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>109</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -293,7 +293,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>61</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -335,7 +335,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1522,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A00893-82C6-4E50-AD7E-57C7467B4A8D}">
   <dimension ref="A4:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1544,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1568,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
experimentos 1 y 2
</commit_message>
<xml_diff>
--- a/Docs importantes/objectives.xlsx
+++ b/Docs importantes/objectives.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Investigacion-maxima-diversidad\Docs importantes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Desktop\Universidad\Cuarto de carrera\Segundo cuatrimestre\Prácticas\Docs importantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D70044-4771-4E24-AC10-2CB411FADB19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACB8598-CCB3-4237-A9C0-577ACEFBDB9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F8ECD58-FE5C-4942-AC5F-309EB15FE9EC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F8ECD58-FE5C-4942-AC5F-309EB15FE9EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Objective counts for pareto solutions:</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>0 MaxSum</t>
   </si>
@@ -56,15 +50,30 @@
   <si>
     <t>4 MinPCenter</t>
   </si>
+  <si>
+    <t>Times</t>
+  </si>
+  <si>
+    <t>Objective functions</t>
+  </si>
+  <si>
+    <t>Objective counts for pareto solutions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,13 +99,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -131,7 +146,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14029435411397351"/>
+          <c:y val="8.3903082806785462E-2"/>
+          <c:w val="0.63907349970861216"/>
+          <c:h val="0.75631856012476351"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -431,7 +456,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -517,7 +542,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -549,7 +574,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="388839248"/>
@@ -591,7 +616,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -628,7 +653,251 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$5:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0 MaxSum</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 MaxMin</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 MaxMinSum</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 MinDiff</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4 MinPCenter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>194736</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-38C3-47C6-A3CA-11091D96FC00}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -679,6 +948,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1182,20 +1491,539 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>33170</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>87349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>33170</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152343</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1215,6 +2043,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>431650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>25436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>216609</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>83034</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98C0944A-D433-4F3B-8FE3-2F6DA5C08171}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1520,64 +2384,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A00893-82C6-4E50-AD7E-57C7467B4A8D}">
-  <dimension ref="A4:B9"/>
+  <dimension ref="A4:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2">
         <v>137</v>
       </c>
+      <c r="C5" s="3">
+        <v>418</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2">
         <v>112</v>
       </c>
+      <c r="C6" s="3">
+        <v>488</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2">
         <v>26</v>
       </c>
+      <c r="C7" s="4">
+        <v>407</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2">
         <v>64</v>
       </c>
+      <c r="C8" s="4">
+        <v>410</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2">
         <v>17</v>
       </c>
+      <c r="C9" s="4">
+        <v>194736</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>